<commit_message>
updated excel file with the insert original method results
</commit_message>
<xml_diff>
--- a/test_results_table_research_question_1/middleware_test_results.xlsx
+++ b/test_results_table_research_question_1/middleware_test_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgedinicola/Desktop/TDRB-Middleware-Extension/test_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgedinicola/Desktop/TDRB-Middleware-Extension/test_results_table_research_question_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D176D3B-15B2-114B-8BD9-C14F5BAE2C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3423CE20-B429-F343-ABEE-5FB48CEF4376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19260" xr2:uid="{BD2E64C6-9971-2049-987A-C9A8CB2241EA}"/>
   </bookViews>
@@ -89,18 +89,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -133,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -145,8 +139,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33AC3783-C63C-AE47-8CCA-EA7F35C5FC8A}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5:R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -498,7 +491,7 @@
       <c r="G4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="I4" s="2" t="s">
@@ -1338,7 +1331,7 @@
         <v>117.675</v>
       </c>
       <c r="H35">
-        <v>121.42</v>
+        <v>127.914</v>
       </c>
       <c r="I35">
         <v>128.69200000000001</v>
@@ -1365,7 +1358,7 @@
         <v>117.547</v>
       </c>
       <c r="H36">
-        <v>127.914</v>
+        <v>128.84200000000001</v>
       </c>
       <c r="I36">
         <v>67.721000000000004</v>
@@ -1392,7 +1385,7 @@
         <v>117.60499999999999</v>
       </c>
       <c r="H37">
-        <v>128.84200000000001</v>
+        <v>120.15900000000001</v>
       </c>
       <c r="I37">
         <v>126.672</v>
@@ -1419,7 +1412,7 @@
         <v>117.907</v>
       </c>
       <c r="H38">
-        <v>120.15900000000001</v>
+        <v>129.10399999999998</v>
       </c>
       <c r="I38">
         <v>65.847999999999999</v>
@@ -1446,7 +1439,7 @@
         <v>117.753</v>
       </c>
       <c r="H39">
-        <v>121.313</v>
+        <v>128.958</v>
       </c>
       <c r="I39">
         <v>184.98099999999999</v>
@@ -1473,7 +1466,7 @@
         <v>117.71299999999999</v>
       </c>
       <c r="H40">
-        <v>129.12</v>
+        <v>129.535</v>
       </c>
       <c r="I40">
         <v>63.198</v>
@@ -1500,7 +1493,7 @@
         <v>117.6</v>
       </c>
       <c r="H41">
-        <v>127.441</v>
+        <v>120.803</v>
       </c>
       <c r="I41">
         <v>121.086</v>
@@ -1526,6 +1519,9 @@
       <c r="G42">
         <v>117.71299999999999</v>
       </c>
+      <c r="H42">
+        <v>122.167</v>
+      </c>
       <c r="I42">
         <v>65.792000000000002</v>
       </c>
@@ -1550,6 +1546,9 @@
       <c r="G43">
         <v>117.675</v>
       </c>
+      <c r="H43">
+        <v>123.51600000000001</v>
+      </c>
       <c r="I43">
         <v>66.787000000000006</v>
       </c>
@@ -1574,7 +1573,9 @@
       <c r="G44" s="3">
         <v>117.30199999999999</v>
       </c>
-      <c r="H44" s="3"/>
+      <c r="H44" s="3">
+        <v>124.818</v>
+      </c>
       <c r="I44" s="3">
         <v>121.95699999999999</v>
       </c>
@@ -1604,9 +1605,9 @@
         <f>AVERAGE(G5:G44)</f>
         <v>117.65675000000002</v>
       </c>
-      <c r="H45" s="12">
+      <c r="H45" s="11">
         <f>AVERAGE(H5:H44)</f>
-        <v>125.04354054054053</v>
+        <v>125.15545</v>
       </c>
       <c r="I45" s="1">
         <f>AVERAGE(I5:I44)</f>

</xml_diff>